<commit_message>
add the function of cal max addr width
</commit_message>
<xml_diff>
--- a/regfile_description.xlsx
+++ b/regfile_description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guodezheng/project/regfile_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBE448B-DF97-7B4B-9FFB-41281F7E07CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0981C2-1BBB-2344-94D3-6D8C7ED3F991}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28120" yWindow="3000" windowWidth="32280" windowHeight="13600" xr2:uid="{20207251-6303-844B-8C58-FFAEC9D786C2}"/>
+    <workbookView xWindow="15060" yWindow="2220" windowWidth="38400" windowHeight="19540" xr2:uid="{20207251-6303-844B-8C58-FFAEC9D786C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>offset</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -146,6 +146,34 @@
   </si>
   <si>
     <t>GPIO0_ODR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Attributes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>descriptions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Module name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gpio_regfile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Base Addr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x40000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data Width</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -204,17 +232,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,207 +558,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5CA718-C1DB-1A4F-BD23-31330EADBFA4}">
-  <dimension ref="A4:AH16"/>
+  <dimension ref="A1:AI16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="3" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:34">
+    <row r="1" spans="1:35">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4">
         <v>31</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>30</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>29</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>28</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>27</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>26</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>25</v>
       </c>
-      <c r="J4">
-        <v>24</v>
-      </c>
       <c r="K4">
+        <v>24</v>
+      </c>
+      <c r="L4">
         <v>23</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>22</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>21</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>20</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>19</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>18</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>17</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>16</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>15</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>14</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>13</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>12</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>11</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>10</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>9</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>8</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>7</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>6</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>5</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>4</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>3</v>
       </c>
-      <c r="AF4">
+      <c r="AG4">
         <v>2</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <v>1</v>
       </c>
-      <c r="AH4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34">
-      <c r="A5" s="1" t="s">
+      <c r="AI4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="1"/>
+      <c r="N5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="1"/>
+      <c r="P5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4" t="s">
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4" t="s">
+      <c r="S5" s="1"/>
+      <c r="T5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4" t="s">
+      <c r="U5" s="1"/>
+      <c r="V5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4" t="s">
+      <c r="W5" s="1"/>
+      <c r="X5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4" t="s">
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="4" t="s">
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="4" t="s">
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="4" t="s">
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AF5" s="4"/>
-      <c r="AG5" s="4" t="s">
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AH5" s="4"/>
-    </row>
-    <row r="6" spans="1:34">
-      <c r="A6" s="2"/>
+      <c r="AI5" s="1"/>
+    </row>
+    <row r="6" spans="1:35">
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
+      <c r="C6" s="2"/>
       <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
       <c r="F6">
         <v>0</v>
       </c>
@@ -738,11 +793,11 @@
         <v>0</v>
       </c>
       <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>1</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
       <c r="J6">
         <v>0</v>
       </c>
@@ -750,11 +805,11 @@
         <v>0</v>
       </c>
       <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
         <v>1</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
       <c r="N6">
         <v>0</v>
       </c>
@@ -762,11 +817,11 @@
         <v>0</v>
       </c>
       <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
         <v>1</v>
       </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
       <c r="R6">
         <v>0</v>
       </c>
@@ -774,11 +829,11 @@
         <v>0</v>
       </c>
       <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
         <v>1</v>
       </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
       <c r="V6">
         <v>0</v>
       </c>
@@ -786,11 +841,11 @@
         <v>0</v>
       </c>
       <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
         <v>1</v>
       </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
       <c r="Z6">
         <v>0</v>
       </c>
@@ -798,11 +853,11 @@
         <v>0</v>
       </c>
       <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
         <v>1</v>
       </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
       <c r="AD6">
         <v>0</v>
       </c>
@@ -810,23 +865,24 @@
         <v>0</v>
       </c>
       <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
         <v>1</v>
       </c>
-      <c r="AG6">
-        <v>0</v>
-      </c>
       <c r="AH6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:34">
-      <c r="A7" s="3"/>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35">
+      <c r="A7" s="2"/>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
+      <c r="C7" s="2"/>
       <c r="D7" t="s">
         <v>24</v>
       </c>
@@ -920,89 +976,105 @@
       <c r="AH7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:34">
-      <c r="A8" s="3" t="s">
+      <c r="AI7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35">
+      <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:34">
-      <c r="A9" s="3"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:35">
+      <c r="A9" s="2"/>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:34">
-      <c r="A10" s="3"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:35">
+      <c r="A10" s="2"/>
       <c r="B10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:34">
-      <c r="A11" s="3" t="s">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:35">
+      <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:34">
-      <c r="A12" s="3"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:35">
+      <c r="A12" s="2"/>
       <c r="B12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:34">
-      <c r="A13" s="3"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:35">
+      <c r="A13" s="2"/>
       <c r="B13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:34">
-      <c r="A14" s="3" t="s">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:35">
+      <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:34">
-      <c r="A15" s="3"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:35">
+      <c r="A15" s="2"/>
       <c r="B15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:34">
-      <c r="A16" s="3"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:35">
+      <c r="A16" s="2"/>
       <c r="B16" t="s">
-        <v>6</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C16" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="AG5:AH5"/>
+  <mergeCells count="24">
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>